<commit_message>
Converted regression problem into classification problem
</commit_message>
<xml_diff>
--- a/a4/Analysis/Linear Regression Performance.xlsx
+++ b/a4/Analysis/Linear Regression Performance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macos-07/Desktop/Files/3_Cornell University/2020-01 Spring/CDS ML Education/IntSys-Education/IntSys-Education/a4/Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37922E10-BC2F-5B4B-9915-03FE3D944773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4398ACA8-790D-074A-A63D-83D263F1CBE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{51CB5DD4-9100-0146-88B6-B6426BFB7C90}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{51CB5DD4-9100-0146-88B6-B6426BFB7C90}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1727,7 +1727,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>